<commit_message>
WiP S400 validated and Electric power variable Pe added
</commit_message>
<xml_diff>
--- a/doc/pumpinfo.xlsx
+++ b/doc/pumpinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DiscoD\Muro\GitHub\multienergysystem\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58892A63-0816-4A31-A85F-C418F79D33C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAA72E3-8F4C-4584-B3C5-7AE9BAD3FD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="683" firstSheet="2" activeTab="10" xr2:uid="{4119C288-BE25-4E3B-9B9B-25A3EA8D7C7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="683" firstSheet="1" activeTab="13" xr2:uid="{4119C288-BE25-4E3B-9B9B-25A3EA8D7C7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36979,16 +36979,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>118696</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>46159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>366347</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>24911</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37017,16 +37017,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>162657</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>178045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>465992</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>61547</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -49842,7 +49842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDB0890-74A7-4484-A5B2-A796C8E2FB71}">
   <dimension ref="AQ6:BI81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AM15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BH37" sqref="BH37"/>
     </sheetView>
   </sheetViews>
@@ -49919,11 +49919,11 @@
         <v>26</v>
       </c>
       <c r="AT15">
-        <f t="shared" ref="AT15:AT23" si="0">-0.039537*AR15*AR15 +0.669933*0.8*AR15 + 24.122662*(0.8*0.8)</f>
+        <f t="shared" ref="AT15:AT20" si="0">-0.039537*AR15*AR15 +0.669933*0.8*AR15 + 24.122662*(0.8*0.8)</f>
         <v>15.724053880000003</v>
       </c>
       <c r="AU15">
-        <f t="shared" ref="AU15:AU19" si="1">-0.039537*AR15*AR15 +0.669933*0.6*AR15 + 24.122662*(0.6*0.6)</f>
+        <f t="shared" ref="AU15:AU18" si="1">-0.039537*AR15*AR15 +0.669933*0.6*AR15 + 24.122662*(0.6*0.6)</f>
         <v>7.2278827199999993</v>
       </c>
       <c r="AV15">
@@ -53134,7 +53134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF412EAB-61E3-4B17-BE4C-3D51DF3A9EED}">
   <dimension ref="A1:AT94"/>
   <sheetViews>
-    <sheetView topLeftCell="J12" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+    <sheetView topLeftCell="C8" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="AE85" sqref="AE85"/>
     </sheetView>
   </sheetViews>
@@ -57620,15 +57620,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494012FD-31C3-43B6-9F73-43D4F1673840}">
-  <dimension ref="F8:G30"/>
+  <dimension ref="F8:H30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>62</v>
       </c>
@@ -57636,31 +57636,43 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F9">
         <v>2.4</v>
       </c>
       <c r="G9">
         <v>9.09</v>
       </c>
+      <c r="H9">
+        <f>-0.041518*F9*F9 + 0.18674*F9 + 8.86824</f>
+        <v>9.0772723200000005</v>
+      </c>
     </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F10">
         <v>3.4</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H18" si="0">-0.041518*F10*F10 + 0.18674*F10 + 8.86824</f>
+        <v>9.0232079200000008</v>
+      </c>
     </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F11">
         <v>5.4</v>
       </c>
       <c r="G11">
         <v>8.6666000000000007</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>8.66597112</v>
+      </c>
     </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F12">
         <v>6</v>
       </c>
@@ -57668,56 +57680,93 @@
         <f>+(8.3333+8.6666)/2</f>
         <v>8.4999500000000001</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>8.4940320000000007</v>
+      </c>
     </row>
-    <row r="13" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F13">
         <v>7.4</v>
       </c>
       <c r="G13">
         <v>8</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>7.9765903199999997</v>
+      </c>
     </row>
-    <row r="14" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F14">
         <v>8.8000000000000007</v>
       </c>
       <c r="G14">
         <v>7.33</v>
       </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>7.2963980799999995</v>
+      </c>
     </row>
-    <row r="15" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F15">
         <v>9.1999999999999993</v>
       </c>
       <c r="G15">
         <v>7</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>7.0721644800000005</v>
+      </c>
     </row>
-    <row r="16" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F16">
         <v>10.4</v>
       </c>
       <c r="G16">
         <v>6.33</v>
       </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>6.31974912</v>
+      </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F17">
         <v>11.8</v>
       </c>
       <c r="G17">
         <v>5.33</v>
       </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>5.2908056799999992</v>
+      </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F18">
         <v>12</v>
       </c>
       <c r="G18">
         <v>5.0999999999999996</v>
       </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>5.130528</v>
+      </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>2.1</v>
+      </c>
+      <c r="H20">
+        <f>-0.041518*F20*F20 + 0.18674*F20 + 8.86824</f>
+        <v>9.0772996199999998</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F22" s="1" t="s">
         <v>62</v>
       </c>
@@ -57725,7 +57774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F23">
         <v>2.4</v>
       </c>
@@ -57733,7 +57782,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F24">
         <v>3.4</v>
       </c>
@@ -57741,7 +57790,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F25">
         <v>4</v>
       </c>
@@ -57749,7 +57798,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F26">
         <v>5.2</v>
       </c>
@@ -57758,7 +57807,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F27">
         <v>6</v>
       </c>
@@ -57766,7 +57815,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F28">
         <v>8.1999999999999993</v>
       </c>
@@ -57774,7 +57823,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F29">
         <v>9.1999999999999993</v>
       </c>
@@ -57783,7 +57832,7 @@
         <v>287.5</v>
       </c>
     </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F30">
         <v>12</v>
       </c>

</xml_diff>